<commit_message>
Change type of 2 resale_flat_txn fields to FLOAT
</commit_message>
<xml_diff>
--- a/Reference/change_history_documentation.xlsx
+++ b/Reference/change_history_documentation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinye\Acodes\JDE\interim project\zz Archive\import data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D830EA6D-603F-4229-817B-B87ACD5EEC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A32403-184B-4882-867E-BAD9FAE4ECA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D5561A44-3570-422D-8B7A-2252C51F3479}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>S102</t>
   </si>
@@ -68,9 +68,6 @@
     <t>1 HDB Town can only get readings from 1 weather station, so Jurong West cannot be mapped to 3 weather stations. Nanyang Avenue was mapped to Jurong West because of its nearest distance.</t>
   </si>
   <si>
-    <t>No HDB town can be mapped; Excluded from locations table</t>
-  </si>
-  <si>
     <t>Remarks</t>
   </si>
   <si>
@@ -80,10 +77,37 @@
     <t>Affected Field Value</t>
   </si>
   <si>
-    <t>No data on air_temp table and humidity table; Excluded from locations table and station table</t>
-  </si>
-  <si>
     <t>Explanation on the mapping of Jurong West, why Tuas South Avenue 3 does not map with any HDB town</t>
+  </si>
+  <si>
+    <t>floor_area_sqm</t>
+  </si>
+  <si>
+    <t>resale_price</t>
+  </si>
+  <si>
+    <t>(n/a)</t>
+  </si>
+  <si>
+    <t>Erica</t>
+  </si>
+  <si>
+    <t>Yvonne</t>
+  </si>
+  <si>
+    <t>Change data type to float, as having ingestion issue via Python</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>No HDB town can be mapped; Included in station table but excluded from locations table</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>No data on air_temp table and humidity table; Included in station table but excluded from locations table</t>
   </si>
 </sst>
 </file>
@@ -169,13 +193,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2941463</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -546,38 +570,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F295524-12FC-46A7-BFCB-B919B2AA6F5B}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" customWidth="1"/>
     <col min="2" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.44140625" customWidth="1"/>
-    <col min="5" max="5" width="106.77734375" customWidth="1"/>
+    <col min="5" max="5" width="83.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45621</v>
       </c>
@@ -591,10 +617,13 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45621</v>
       </c>
@@ -602,39 +631,82 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>45621</v>
+        <v>45622</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45622</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45622</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>